<commit_message>
Testing code additions Still in development
</commit_message>
<xml_diff>
--- a/ProgramFiles/config_files/1 - CDP Network Audit _ Template.xlsx
+++ b/ProgramFiles/config_files/1 - CDP Network Audit _ Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\PycharmProjects\AsyncSSH\config_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python\Pycharm Projects\CDP_Network_Audit-AsyncSSH\ProgramFiles\config_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3D14995-A9D6-47B2-B300-E4CCC6301CF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{435153BA-F3D2-40C9-AEC2-BBE5C7546121}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Audit" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t>CDP Device Audit</t>
   </si>
@@ -41,9 +41,6 @@
     <t>Time:</t>
   </si>
   <si>
-    <t>10.145.63.1</t>
-  </si>
-  <si>
     <t>LOCAL_HOST</t>
   </si>
   <si>
@@ -71,21 +68,6 @@
     <t>CAPABILITIES</t>
   </si>
   <si>
-    <t>GB-CAY2-001CSW001</t>
-  </si>
-  <si>
-    <t>GB-CAY2-001ASW001</t>
-  </si>
-  <si>
-    <t>10.145.61.10</t>
-  </si>
-  <si>
-    <t>gb-cay2-001sdw101</t>
-  </si>
-  <si>
-    <t>gb-cay2-001sdw102</t>
-  </si>
-  <si>
     <t>Reverse DNS Lookup</t>
   </si>
   <si>
@@ -93,12 +75,6 @@
   </si>
   <si>
     <t>IP Address</t>
-  </si>
-  <si>
-    <t>10.255.145.61</t>
-  </si>
-  <si>
-    <t>10.255.145.62</t>
   </si>
   <si>
     <t>Connection Errors</t>
@@ -331,7 +307,7 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -406,15 +382,18 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -447,9 +426,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -487,9 +466,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -522,9 +501,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -557,9 +553,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -736,20 +749,20 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="30.6640625" customWidth="1"/>
-    <col min="4" max="4" width="50.6640625" customWidth="1"/>
-    <col min="5" max="5" width="38.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="30.6640625" customWidth="1"/>
-    <col min="10" max="10" width="108.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="50.7109375" customWidth="1"/>
+    <col min="5" max="5" width="38.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="30.7109375" customWidth="1"/>
+    <col min="10" max="10" width="108.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="27.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
@@ -763,7 +776,7 @@
       <c r="I1" s="24"/>
       <c r="J1" s="24"/>
     </row>
-    <row r="2" spans="1:11" s="2" customFormat="1" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" s="2" customFormat="1" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="23"/>
       <c r="B2" s="21"/>
       <c r="C2" s="21"/>
@@ -775,49 +788,49 @@
       <c r="I2" s="23"/>
       <c r="J2" s="23"/>
     </row>
-    <row r="3" spans="1:11" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="4"/>
     </row>
-    <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="4"/>
     </row>
-    <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="4"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B7" s="4"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="B8" s="4"/>
     </row>
-    <row r="9" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6"/>
       <c r="B9" s="4"/>
     </row>
-    <row r="10" spans="1:11" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="14" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B10" s="15"/>
       <c r="C10" s="15"/>
       <c r="D10" s="15"/>
       <c r="E10" s="16"/>
       <c r="F10" s="17" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="G10" s="18"/>
       <c r="H10" s="18"/>
@@ -825,39 +838,39 @@
       <c r="J10" s="18"/>
       <c r="K10" s="19"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="C11" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="D11" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="E11" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="F11" s="13" t="s">
+      <c r="G11" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="G11" s="13" t="s">
+      <c r="H11" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="H11" s="13" t="s">
+      <c r="I11" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="I11" s="13" t="s">
+      <c r="J11" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="J11" s="13" t="s">
+      <c r="K11" s="13" t="s">
         <v>12</v>
-      </c>
-      <c r="K11" s="13" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -883,67 +896,35 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.6640625" customWidth="1"/>
-    <col min="2" max="2" width="25.6640625" customWidth="1"/>
+    <col min="1" max="1" width="35.7109375" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="s">
-        <v>19</v>
+    <row r="1" spans="1:2" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="29" t="s">
+        <v>13</v>
       </c>
       <c r="B1" s="25"/>
     </row>
-    <row r="2" spans="1:2" s="8" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="23"/>
+    <row r="2" spans="1:2" s="8" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="30"/>
       <c r="B2" s="23"/>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
         <v>15</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -966,28 +947,28 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="28"/>
-    </row>
-    <row r="2" spans="1:2" s="10" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="27"/>
+    </row>
+    <row r="2" spans="1:2" s="10" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="23"/>
       <c r="B2" s="23"/>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -1003,28 +984,28 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="B1" s="28"/>
-    </row>
-    <row r="2" spans="1:2" s="12" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="27"/>
+    </row>
+    <row r="2" spans="1:2" s="12" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="23"/>
       <c r="B2" s="23"/>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added section in to save connection errors to the spreadsheet
</commit_message>
<xml_diff>
--- a/ProgramFiles/config_files/1 - CDP Network Audit _ Template.xlsx
+++ b/ProgramFiles/config_files/1 - CDP Network Audit _ Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python\Pycharm Projects\CDP_Network_Audit-AsyncSSH\ProgramFiles\config_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{517A0DC7-029D-47E3-B6D5-625ABAA1B827}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7321B90A-F50A-40CB-A7FC-3FD79416EC4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>Site Code:</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>CDP Network Audit</t>
+  </si>
+  <si>
+    <t>Error</t>
   </si>
 </sst>
 </file>
@@ -301,7 +304,7 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -366,9 +369,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -376,18 +376,18 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -710,7 +710,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="11" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -722,28 +722,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="23" t="s">
         <v>20</v>
       </c>
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="23"/>
+      <c r="A2" s="29"/>
       <c r="B2" s="21"/>
       <c r="C2" s="21"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
     </row>
     <row r="3" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -857,14 +857,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="25"/>
+      <c r="B1" s="24"/>
     </row>
     <row r="2" spans="1:2" s="8" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="27"/>
-      <c r="B2" s="23"/>
+      <c r="A2" s="29"/>
+      <c r="B2" s="22"/>
     </row>
     <row r="3" spans="1:2" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -900,23 +900,26 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="1" max="2" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="29"/>
+      <c r="B1" s="26"/>
     </row>
     <row r="2" spans="1:2" s="10" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="23"/>
-      <c r="B2" s="23"/>
+      <c r="A2" s="22"/>
+      <c r="B2" s="22"/>
     </row>
     <row r="3" spans="1:2" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>12</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -932,7 +935,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T1" sqref="T1"/>
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -941,14 +944,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="29"/>
+      <c r="B1" s="26"/>
     </row>
     <row r="2" spans="1:2" s="12" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="23"/>
-      <c r="B2" s="23"/>
+      <c r="A2" s="22"/>
+      <c r="B2" s="22"/>
     </row>
     <row r="3" spans="1:2" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
- Resolved bug with recursion
</commit_message>
<xml_diff>
--- a/ProgramFiles/config_files/1 - CDP Network Audit _ Template.xlsx
+++ b/ProgramFiles/config_files/1 - CDP Network Audit _ Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python\Pycharm Projects\CDP_Network_Audit-AsyncSSH\ProgramFiles\config_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7321B90A-F50A-40CB-A7FC-3FD79416EC4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2242A986-9D24-4067-AD1B-ED8BAC32EC7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t>Site Code:</t>
   </si>
@@ -86,13 +86,16 @@
     <t>Remote Host Information</t>
   </si>
   <si>
-    <t>Seed Device:</t>
-  </si>
-  <si>
     <t>CDP Network Audit</t>
   </si>
   <si>
     <t>Error</t>
+  </si>
+  <si>
+    <t>Seed Device 1:</t>
+  </si>
+  <si>
+    <t>Seed Device 2:</t>
   </si>
 </sst>
 </file>
@@ -369,12 +372,18 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -382,12 +391,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -710,7 +713,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="11" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -722,28 +725,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
-        <v>20</v>
+      <c r="A1" s="22" t="s">
+        <v>19</v>
       </c>
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="29"/>
+      <c r="A2" s="23"/>
       <c r="B2" s="21"/>
       <c r="C2" s="21"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
     </row>
     <row r="3" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -766,12 +769,14 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B7" s="4"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
+      <c r="A8" s="6" t="s">
+        <v>22</v>
+      </c>
       <c r="B8" s="4"/>
     </row>
     <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -857,14 +862,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="24"/>
+      <c r="B1" s="25"/>
     </row>
     <row r="2" spans="1:2" s="8" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="29"/>
-      <c r="B2" s="22"/>
+      <c r="A2" s="23"/>
+      <c r="B2" s="24"/>
     </row>
     <row r="3" spans="1:2" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -904,14 +909,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="26"/>
+      <c r="B1" s="28"/>
     </row>
     <row r="2" spans="1:2" s="10" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="22"/>
-      <c r="B2" s="22"/>
+      <c r="A2" s="24"/>
+      <c r="B2" s="24"/>
     </row>
     <row r="3" spans="1:2" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -919,7 +924,7 @@
         <v>12</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -944,14 +949,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="26"/>
+      <c r="B1" s="28"/>
     </row>
     <row r="2" spans="1:2" s="12" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="22"/>
-      <c r="B2" s="22"/>
+      <c r="A2" s="24"/>
+      <c r="B2" s="24"/>
     </row>
     <row r="3" spans="1:2" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>